<commit_message>
Métodos introducidos en el .ppt
</commit_message>
<xml_diff>
--- a/Ficheros/Soluciones.xlsx
+++ b/Ficheros/Soluciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SAGEMath\MASI\Ficheros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7362FF69-8E70-4DA9-96EC-BFCACD462C4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2392D204-5047-4383-8F0F-D27B059B1EEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="480" windowWidth="25870" windowHeight="18340" activeTab="2" xr2:uid="{8C5FD1BC-D174-4370-BFAB-40543485D895}"/>
+    <workbookView xWindow="8500" yWindow="1380" windowWidth="25870" windowHeight="18340" activeTab="1" xr2:uid="{8C5FD1BC-D174-4370-BFAB-40543485D895}"/>
   </bookViews>
   <sheets>
     <sheet name="North-West Method" sheetId="1" r:id="rId1"/>
@@ -2461,8 +2461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36448D51-4F37-48DE-A54A-4E69FBBFF396}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73:G82"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3906,7 +3906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BA3B73E-54D1-418D-B20A-9668680A1AAD}">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G91" sqref="A82:G91"/>
     </sheetView>
   </sheetViews>

</xml_diff>